<commit_message>
added: weight files, val_datasets, info files, sheet of outputs images
</commit_message>
<xml_diff>
--- a/test_results/test_results.xlsx
+++ b/test_results/test_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janbu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janbu\PycharmProjects\PracaMagisterska\test_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35420BDC-E463-4188-B32F-B7CC85F6B02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD791CD8-4E33-471C-9124-6100641709F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="2310" windowWidth="38640" windowHeight="15840" xr2:uid="{F258C1A5-C34B-49C9-8B9F-0E9C8BEDBED8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
   <si>
     <t>loss</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>test rhythmic acc</t>
+  </si>
+  <si>
+    <t>wyniki dla najlepszego val loss</t>
   </si>
 </sst>
 </file>
@@ -85,7 +88,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -104,12 +107,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -127,8 +136,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -435,7 +444,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -443,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528529D1-E348-40B3-8F44-95294D5DB6F6}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,315 +503,312 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2">
         <v>50</v>
       </c>
-      <c r="C2" s="2">
-        <v>300</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.35980000000000001</v>
-      </c>
-      <c r="E2" s="3">
-        <v>5.3516000000000004</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0.91490000000000005</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0.50309999999999999</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0.96960000000000002</v>
-      </c>
-      <c r="I2" s="3">
-        <v>0.76349999999999996</v>
+      <c r="C2">
+        <v>300</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="E2" s="2">
+        <v>4.4630000000000001</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.79600000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>100</v>
       </c>
-      <c r="C3" s="2">
-        <v>300</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.2288</v>
-      </c>
-      <c r="E3" s="3">
-        <v>5.7770000000000001</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0.94699999999999995</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0.51800000000000002</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0.98099999999999998</v>
-      </c>
-      <c r="I3" s="3">
-        <v>0.77400000000000002</v>
+      <c r="C3">
+        <v>300</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4.7990000000000004</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.79800000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>50</v>
       </c>
-      <c r="C4" s="2">
-        <v>300</v>
-      </c>
-      <c r="D4" s="3">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="E4" s="3">
-        <v>5.96</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="C4">
+        <v>300</v>
+      </c>
+      <c r="D4" s="2">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4.8869999999999996</v>
+      </c>
+      <c r="F4" s="2">
         <v>0.97499999999999998</v>
       </c>
-      <c r="G4" s="3">
-        <v>0.57699999999999996</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0.995</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0.85199999999999998</v>
+      <c r="G4" s="2">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.878</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>100</v>
       </c>
-      <c r="C5" s="2">
-        <v>300</v>
-      </c>
-      <c r="D5" s="3">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="E5" s="3">
-        <v>5.9640000000000004</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0.55500000000000005</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0.99299999999999999</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0.84599999999999997</v>
+      <c r="C5">
+        <v>300</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4.3620000000000001</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.94279999999999997</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.63339999999999996</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.879</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>50</v>
       </c>
-      <c r="C6" s="2">
-        <v>300</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.126</v>
-      </c>
-      <c r="E6" s="3">
-        <v>6.5819999999999999</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.97199999999999998</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.60099999999999998</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.98799999999999999</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0.77300000000000002</v>
+      <c r="C6">
+        <v>300</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5.5519999999999996</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.64</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.79600000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7">
         <v>100</v>
       </c>
-      <c r="C7" s="2">
-        <v>300</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0.11899999999999999</v>
-      </c>
-      <c r="E7" s="3">
-        <v>7.0860000000000003</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0.57899999999999996</v>
-      </c>
-      <c r="H7" s="3">
+      <c r="C7">
+        <v>300</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="E7" s="2">
+        <v>6.3949999999999996</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="H7" s="2">
         <v>0.98799999999999999</v>
       </c>
-      <c r="I7" s="3">
-        <v>0.75849999999999995</v>
+      <c r="I7" s="2">
+        <v>0.77900000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8">
         <v>50</v>
       </c>
-      <c r="C8" s="2">
-        <v>300</v>
-      </c>
-      <c r="D8" s="3">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="E8" s="3">
-        <v>2.8929999999999998</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0.98599999999999999</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0.73899999999999999</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0.99299999999999999</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0.89300000000000002</v>
+      <c r="C8">
+        <v>300</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2.3090000000000002</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.996</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.90900000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B9">
         <v>100</v>
       </c>
-      <c r="C9" s="2">
-        <v>300</v>
-      </c>
-      <c r="D9" s="3">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="E9" s="3">
-        <v>3.0609999999999999</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0.98899999999999999</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0.70899999999999996</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0.995</v>
-      </c>
-      <c r="I9" s="3">
-        <v>0.88800000000000001</v>
+      <c r="C9">
+        <v>300</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2.5771999999999999</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.91500000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B10">
         <v>50</v>
       </c>
-      <c r="C10" s="2">
-        <v>300</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0.216</v>
-      </c>
-      <c r="E10" s="3">
-        <v>5.0140000000000002</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0.94899999999999995</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0.47399999999999998</v>
-      </c>
-      <c r="H10" s="3">
-        <v>0.97799999999999998</v>
-      </c>
-      <c r="I10" s="3">
-        <v>0.73799999999999999</v>
+      <c r="C10">
+        <v>300</v>
+      </c>
+      <c r="D10" s="2">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>50.070999999999998</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.745</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B11">
         <v>100</v>
       </c>
-      <c r="C11" s="2">
-        <v>300</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="E11" s="3">
-        <v>4.843</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0.95099999999999996</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0.47899999999999998</v>
-      </c>
-      <c r="H11" s="3">
-        <v>0.98</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0.73199999999999998</v>
+      <c r="C11">
+        <v>300</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4.992</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.752</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="2"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -811,7 +817,9 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="2"/>
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -820,7 +828,6 @@
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="2"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -828,68 +835,324 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C17" s="2"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C18" s="2"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C19" s="2"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>50</v>
+      </c>
+      <c r="C18">
+        <v>300</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1.6359999999999999</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2.931</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.6089</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>100</v>
+      </c>
+      <c r="C19">
+        <v>300</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1.952</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.30248000000000003</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.53769999999999996</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.78439999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>50</v>
+      </c>
+      <c r="C20">
+        <v>300</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1.456</v>
+      </c>
+      <c r="E20" s="2">
+        <v>3.0070000000000001</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.629</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>100</v>
+      </c>
+      <c r="C21">
+        <v>300</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1.6639999999999999</v>
+      </c>
+      <c r="E21" s="2">
+        <v>2.9889999999999999</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.85299999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>50</v>
+      </c>
+      <c r="C22">
+        <v>300</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1.847</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3.4630000000000001</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0.77100000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>100</v>
+      </c>
+      <c r="C23">
+        <v>300</v>
+      </c>
+      <c r="D23" s="2">
+        <v>2.0449999999999999</v>
+      </c>
+      <c r="E23" s="2">
+        <v>3.7160000000000002</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0.746</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>50</v>
+      </c>
+      <c r="C24">
+        <v>300</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1.681</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.745</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>100</v>
+      </c>
+      <c r="C25">
+        <v>300</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1.7669999999999999</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0.90600000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <v>50</v>
+      </c>
+      <c r="C26">
+        <v>300</v>
+      </c>
+      <c r="D26" s="2">
+        <v>2.0110000000000001</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2.5569999999999999</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0.748</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>100</v>
+      </c>
+      <c r="C27">
+        <v>300</v>
+      </c>
+      <c r="D27" s="2">
+        <v>2.1269999999999998</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2.6320000000000001</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0.73599999999999999</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>